<commit_message>
populated several goals in prep with data
</commit_message>
<xml_diff>
--- a/prep/FIS/HH_fish.xlsx
+++ b/prep/FIS/HH_fish.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="-165" windowWidth="27555" windowHeight="13065"/>
+    <workbookView xWindow="3390" yWindow="225" windowWidth="27555" windowHeight="13065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,10 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="9">
-  <si>
-    <t>YEAR</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="8">
   <si>
     <t>Kauai</t>
   </si>
@@ -30,19 +27,19 @@
     <t>Hawaii</t>
   </si>
   <si>
-    <t>Rgn_ID</t>
-  </si>
-  <si>
-    <t>Rgn_Name</t>
-  </si>
-  <si>
     <t>Maui Nui</t>
   </si>
   <si>
-    <t>Percent_households_fish</t>
+    <t>rng_id</t>
   </si>
   <si>
-    <t>Weight by population to get need by island?</t>
+    <t>rgn_name</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>percent_households_fish</t>
   </si>
 </sst>
 </file>
@@ -381,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,7 +389,7 @@
     <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -400,21 +397,18 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>2004</v>
@@ -423,12 +417,12 @@
         <v>14.1966562765656</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2005</v>
@@ -437,12 +431,12 @@
         <v>13.184584178498987</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>2006</v>
@@ -451,12 +445,12 @@
         <v>14.678624813153963</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>2007</v>
@@ -465,12 +459,12 @@
         <v>14.140127388535031</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>2008</v>
@@ -479,12 +473,12 @@
         <v>13.812858052196052</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>2009</v>
@@ -493,12 +487,12 @@
         <v>14.358647096362475</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>2010</v>
@@ -507,12 +501,12 @@
         <v>12.966537966537967</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>2011</v>
@@ -521,12 +515,12 @@
         <v>10.665362035225048</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>2012</v>
@@ -535,12 +529,12 @@
         <v>10.291197882197221</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>2013</v>
@@ -549,12 +543,12 @@
         <v>9.6987752399867588</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C12">
         <v>2004</v>
@@ -563,12 +557,12 @@
         <v>17.389575694668665</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>2005</v>
@@ -577,12 +571,12 @@
         <v>17.525493917144342</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>2006</v>
@@ -591,12 +585,12 @@
         <v>21.538901712292567</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>2007</v>
@@ -605,12 +599,12 @@
         <v>19.125089649386322</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>2008</v>
@@ -624,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>2009</v>
@@ -638,7 +632,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>2010</v>
@@ -652,7 +646,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>2011</v>
@@ -666,7 +660,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C20">
         <v>2012</v>
@@ -680,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>2013</v>
@@ -694,7 +688,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <v>2004</v>
@@ -708,7 +702,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>2005</v>
@@ -722,7 +716,7 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>2006</v>
@@ -736,7 +730,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25">
         <v>2007</v>
@@ -750,7 +744,7 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>2008</v>
@@ -764,7 +758,7 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>2009</v>
@@ -778,7 +772,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>2010</v>
@@ -792,7 +786,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <v>2011</v>
@@ -806,7 +800,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>2012</v>
@@ -820,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31">
         <v>2013</v>
@@ -834,7 +828,7 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C32">
         <v>2004</v>
@@ -848,7 +842,7 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33">
         <v>2005</v>
@@ -862,7 +856,7 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34">
         <v>2006</v>
@@ -876,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35">
         <v>2007</v>
@@ -890,7 +884,7 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <v>2008</v>
@@ -904,7 +898,7 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37">
         <v>2009</v>
@@ -918,7 +912,7 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38">
         <v>2010</v>
@@ -932,7 +926,7 @@
         <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39">
         <v>2011</v>
@@ -946,7 +940,7 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40">
         <v>2012</v>
@@ -960,7 +954,7 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C41">
         <v>2013</v>

</xml_diff>